<commit_message>
removed unneeded if statement
</commit_message>
<xml_diff>
--- a/data/alignments/constant_tempo.xlsx
+++ b/data/alignments/constant_tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtjor\OneDrive - purdue.edu\Documents\Purdue-Artificial-Intelligence-in-Music\Companion-code\data\alignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4B3867-07A2-4CC7-813E-405465124EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CFDF08-0642-4BD7-AA56-D43B16B089CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Merge accompaniment error into main (#63)
* added alignment error template

* split alignment files

* updated template

* made function to calculate accompaniment error

* removed unneeded if statement

---------

Co-authored-by: Ryan Jordan <34822768+rtjord@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/alignments/constant_tempo.xlsx
+++ b/data/alignments/constant_tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtjor\OneDrive - purdue.edu\Documents\Purdue-Artificial-Intelligence-in-Music\Companion-code\data\alignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE1355C-A7A0-428E-83BD-5BEA31CB94E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CFDF08-0642-4BD7-AA56-D43B16B089CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>